<commit_message>
Fixes #35 , Fixes #32
</commit_message>
<xml_diff>
--- a/tests/fixtures_files/fs-ZamoraEsteban.xlsx
+++ b/tests/fixtures_files/fs-ZamoraEsteban.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t xml:space="preserve">offset=0 count=75 +surname:zamora~ +father_givenname:juan~ +mother_givenname:lorenza~ +mother_surname:estaban~ +record_country:Spain acl=(CdsPrmAnyone+or+CdsPrmRegisteredPatron) </t>
   </si>
@@ -144,24 +144,6 @@
     <t>ark:/61903/1:1:F52T-Z2B</t>
   </si>
   <si>
-    <t>Elena Zamora Esteban</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>17 Aug 1860</t>
-  </si>
-  <si>
-    <t>25 Aug 1860</t>
-  </si>
-  <si>
-    <t>1860</t>
-  </si>
-  <si>
-    <t>ark:/61903/1:1:F5G6-48Z</t>
-  </si>
-  <si>
     <t>15 Jul 1851</t>
   </si>
   <si>
@@ -174,21 +156,6 @@
     <t>ark:/61903/1:1:F5G6-ZXP</t>
   </si>
   <si>
-    <t>Mariano Zamora Esteban</t>
-  </si>
-  <si>
-    <t>26 Jul 1855</t>
-  </si>
-  <si>
-    <t>29 Jul 1855</t>
-  </si>
-  <si>
-    <t>1855</t>
-  </si>
-  <si>
-    <t>ark:/61903/1:1:F5G6-N86</t>
-  </si>
-  <si>
     <t>Enrique Zamora Esteban</t>
   </si>
   <si>
@@ -202,39 +169,6 @@
   </si>
   <si>
     <t>Manuel Toral;Fermina Martin</t>
-  </si>
-  <si>
-    <t>Tiburcio Zamora Esteban</t>
-  </si>
-  <si>
-    <t>14 Apr 1866</t>
-  </si>
-  <si>
-    <t>20 Apr 1866</t>
-  </si>
-  <si>
-    <t>1866</t>
-  </si>
-  <si>
-    <t>C87384-8</t>
-  </si>
-  <si>
-    <t>ark:/61903/1:1:F52R-189</t>
-  </si>
-  <si>
-    <t>Toribia Zamora Esteban</t>
-  </si>
-  <si>
-    <t>27 Apr 1863</t>
-  </si>
-  <si>
-    <t>03 May 1863</t>
-  </si>
-  <si>
-    <t>1863</t>
-  </si>
-  <si>
-    <t>ark:/61903/1:1:FRMD-657</t>
   </si>
   <si>
     <t>22 Mar 1879</t>
@@ -251,30 +185,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
@@ -319,17 +233,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AA12"/>
+  <dimension ref="A2:AA8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="A9" sqref="A9:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -740,10 +650,10 @@
         <v>35</v>
       </c>
       <c r="J7" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="P7" t="s">
         <v>36</v>
@@ -752,10 +662,10 @@
         <v>37</v>
       </c>
       <c r="R7" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="T7" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="V7" t="s">
         <v>38</v>
@@ -772,32 +682,44 @@
         <v>7.4900007247924805</v>
       </c>
       <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
         <v>42</v>
-      </c>
-      <c r="D8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" t="s">
-        <v>44</v>
       </c>
       <c r="G8" t="s">
         <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I8" t="s">
         <v>35</v>
       </c>
+      <c r="J8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" t="s">
+        <v>47</v>
+      </c>
       <c r="P8" t="s">
         <v>36</v>
       </c>
       <c r="Q8" t="s">
         <v>37</v>
       </c>
+      <c r="R8" t="s">
+        <v>48</v>
+      </c>
+      <c r="T8" t="s">
+        <v>49</v>
+      </c>
       <c r="V8" t="s">
         <v>38</v>
       </c>
@@ -805,195 +727,15 @@
         <v>39</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>7.4900007247924805</v>
-      </c>
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" t="s">
-        <v>57</v>
-      </c>
-      <c r="K9" t="s">
-        <v>58</v>
-      </c>
-      <c r="P9" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>37</v>
-      </c>
-      <c r="R9" t="s">
-        <v>59</v>
-      </c>
-      <c r="T9" t="s">
-        <v>60</v>
-      </c>
-      <c r="V9" t="s">
-        <v>38</v>
-      </c>
-      <c r="X9" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z9" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>7.4900007247924805</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" t="s">
-        <v>35</v>
-      </c>
-      <c r="P10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>37</v>
-      </c>
-      <c r="V10" t="s">
-        <v>38</v>
-      </c>
-      <c r="X10" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z10" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>6.7700004577636719</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" t="s">
-        <v>35</v>
-      </c>
-      <c r="P11" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>37</v>
-      </c>
-      <c r="V11" t="s">
-        <v>65</v>
-      </c>
-      <c r="X11" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z11" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>6.7700004577636719</v>
-      </c>
-      <c r="B12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I12" t="s">
-        <v>35</v>
-      </c>
-      <c r="P12" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>37</v>
-      </c>
-      <c r="V12" t="s">
-        <v>65</v>
-      </c>
-      <c r="X12" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z12" s="9" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="url"/>
+    <hyperlink ref="A2" r:id="rId1" location="&amp;offset=0&amp;count=75&amp;query=+surname:zamora~ +father_givenname:juan~ +mother_givenname:lorenza~ +mother_surname:estaban~ +record_country:Spain &amp;acl=(CdsPrmAnyone+or+CdsPrmRegisteredPatron)" display="url"/>
     <hyperlink ref="Z6" r:id="rId2" display="url"/>
     <hyperlink ref="Z7" r:id="rId3" display="url"/>
     <hyperlink ref="Z8" r:id="rId4" display="url"/>
-    <hyperlink ref="Z9" r:id="rId5" display="url"/>
-    <hyperlink ref="Z10" r:id="rId6" display="url"/>
-    <hyperlink ref="Z11" r:id="rId7" display="url"/>
-    <hyperlink ref="Z12" r:id="rId8" display="url"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>